<commit_message>
contains values for PPDs for stellar population modeling
</commit_message>
<xml_diff>
--- a/hst/PROSPECTOR/Results worksheet for stellar mass, age, and dust.xlsx
+++ b/hst/PROSPECTOR/Results worksheet for stellar mass, age, and dust.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="460" windowWidth="19680" windowHeight="18940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Mass" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="49">
   <si>
     <t>J0826</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Galaxy</t>
   </si>
   <si>
-    <t>Best Mass</t>
-  </si>
-  <si>
     <t>Upper Limit</t>
   </si>
   <si>
@@ -107,6 +104,78 @@
   </si>
   <si>
     <t>Best Dust</t>
+  </si>
+  <si>
+    <t>SSP Best Mass</t>
+  </si>
+  <si>
+    <t>Tau Best Mass</t>
+  </si>
+  <si>
+    <t>DTau Best Mass</t>
+  </si>
+  <si>
+    <t>SSP Lo Unc</t>
+  </si>
+  <si>
+    <t>Calz Best Mass</t>
+  </si>
+  <si>
+    <t>SSP Up Unc</t>
+  </si>
+  <si>
+    <t>Cal Up Unc</t>
+  </si>
+  <si>
+    <t>Tau Up Unc</t>
+  </si>
+  <si>
+    <t>DTau Up Unc</t>
+  </si>
+  <si>
+    <t>Cal Lo Unc</t>
+  </si>
+  <si>
+    <t>tau Lo Unc</t>
+  </si>
+  <si>
+    <t>dtau lo unc</t>
+  </si>
+  <si>
+    <t>SSP 16th %</t>
+  </si>
+  <si>
+    <t>Cal 16th %</t>
+  </si>
+  <si>
+    <t>Tau 16th %</t>
+  </si>
+  <si>
+    <t>DTau 16th %</t>
+  </si>
+  <si>
+    <t>SSP 50th %</t>
+  </si>
+  <si>
+    <t>cal 50th %</t>
+  </si>
+  <si>
+    <t>tau 50th %</t>
+  </si>
+  <si>
+    <t>dtau 50th %</t>
+  </si>
+  <si>
+    <t>SSP 84th %</t>
+  </si>
+  <si>
+    <t>cal 84th %</t>
+  </si>
+  <si>
+    <t>tau 84th %</t>
+  </si>
+  <si>
+    <t>dtau 84th %</t>
   </si>
 </sst>
 </file>
@@ -421,1182 +490,1034 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I61"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>12397862400</v>
+      </c>
+      <c r="C2">
+        <v>11725326336</v>
+      </c>
+      <c r="D2">
+        <v>5561881856</v>
+      </c>
+      <c r="E2">
+        <v>6035295488</v>
+      </c>
+      <c r="F2">
+        <v>1991570329</v>
+      </c>
+      <c r="G2">
+        <v>2014845132.8</v>
+      </c>
+      <c r="H2">
+        <v>3549309696</v>
+      </c>
+      <c r="I2">
+        <v>1691007846.4000001</v>
+      </c>
+      <c r="J2">
+        <v>1700643328</v>
+      </c>
+      <c r="K2">
+        <v>4564549</v>
+      </c>
+      <c r="L2">
+        <v>1298802944</v>
+      </c>
+      <c r="M2">
+        <v>1047843993.6</v>
+      </c>
+      <c r="N2">
+        <v>10697219072</v>
+      </c>
+      <c r="O2">
+        <v>7160777216</v>
+      </c>
+      <c r="P2">
+        <v>4263078912</v>
+      </c>
+      <c r="Q2">
+        <v>4987451494.3999996</v>
+      </c>
+      <c r="R2">
+        <v>12397862400</v>
+      </c>
+      <c r="S2">
+        <v>11725326336</v>
+      </c>
+      <c r="T2">
+        <v>5561881856</v>
+      </c>
+      <c r="U2">
+        <v>6035295488</v>
+      </c>
+      <c r="V2">
+        <v>14389432729.6</v>
+      </c>
+      <c r="W2">
+        <v>13740171468.799999</v>
+      </c>
+      <c r="X2">
+        <v>9111191552</v>
+      </c>
+      <c r="Y2">
+        <v>772630334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8692855808</v>
+      </c>
+      <c r="C3">
+        <v>14480795648</v>
       </c>
       <c r="D3">
-        <v>12397862400</v>
+        <v>5923102720</v>
       </c>
       <c r="E3">
-        <v>1991570329</v>
+        <v>6038848512</v>
       </c>
       <c r="F3">
-        <v>1700643328</v>
+        <v>2828185600</v>
       </c>
       <c r="G3">
-        <v>10697219072</v>
+        <v>3204681728</v>
       </c>
       <c r="H3">
-        <v>12397862400</v>
+        <v>3335118848</v>
       </c>
       <c r="I3">
-        <v>14389432729.6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>14</v>
+        <v>1656857190.4000001</v>
+      </c>
+      <c r="J3">
+        <v>2009430016</v>
+      </c>
+      <c r="K3">
+        <v>6328422528</v>
+      </c>
+      <c r="L3">
+        <v>1591776526</v>
+      </c>
+      <c r="M3">
+        <v>1012921856</v>
+      </c>
+      <c r="N3">
+        <v>6683425792</v>
+      </c>
+      <c r="O3">
+        <v>8162373120</v>
+      </c>
+      <c r="P3">
+        <v>4331326464</v>
+      </c>
+      <c r="Q3">
+        <v>5025926656</v>
+      </c>
+      <c r="R3">
+        <v>8692855808</v>
+      </c>
+      <c r="S3">
+        <v>14480795648</v>
+      </c>
+      <c r="T3">
+        <v>5923102720</v>
+      </c>
+      <c r="U3">
+        <v>6038848512</v>
+      </c>
+      <c r="V3">
+        <v>11521041408</v>
+      </c>
+      <c r="W3">
+        <v>17685477376</v>
+      </c>
+      <c r="X3">
+        <v>9258221568</v>
+      </c>
+      <c r="Y3">
+        <v>7695705702.3999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>12349798400</v>
+      </c>
+      <c r="C4">
+        <v>2680420608</v>
       </c>
       <c r="D4">
-        <v>11725326336</v>
+        <v>5790441472</v>
       </c>
       <c r="E4">
-        <v>2014845132.8</v>
+        <v>6081265664</v>
       </c>
       <c r="F4">
-        <v>4564549</v>
+        <v>1978885120</v>
       </c>
       <c r="G4">
-        <v>7160777216</v>
+        <v>8086517504</v>
       </c>
       <c r="H4">
-        <v>11725326336</v>
+        <v>3468123340.8000002</v>
       </c>
       <c r="I4">
-        <v>13740171468.799999</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>15</v>
+        <v>1648764313.5999999</v>
+      </c>
+      <c r="J4">
+        <v>1746161049.5999999</v>
+      </c>
+      <c r="K4">
+        <v>546768768</v>
+      </c>
+      <c r="L4">
+        <v>1514427904</v>
+      </c>
+      <c r="M4">
+        <v>1057875456</v>
+      </c>
+      <c r="N4">
+        <v>10603637350.4</v>
+      </c>
+      <c r="O4">
+        <v>2133651840</v>
+      </c>
+      <c r="P4">
+        <v>4276013568</v>
+      </c>
+      <c r="Q4">
+        <v>5023390208</v>
+      </c>
+      <c r="R4">
+        <v>12349798400</v>
+      </c>
+      <c r="S4">
+        <v>2680420608</v>
+      </c>
+      <c r="T4">
+        <v>5790441472</v>
+      </c>
+      <c r="U4">
+        <v>6081265664</v>
+      </c>
+      <c r="V4">
+        <v>14328683520</v>
+      </c>
+      <c r="W4">
+        <v>10766938112</v>
+      </c>
+      <c r="X4">
+        <v>9258564812.7999992</v>
+      </c>
+      <c r="Y4">
+        <v>7730029977.6000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>12374023680</v>
+      </c>
+      <c r="C5">
+        <v>12626169856</v>
       </c>
       <c r="D5">
-        <v>5561881856</v>
+        <v>5527543808</v>
       </c>
       <c r="E5">
-        <v>3549309696</v>
+        <v>6122680064</v>
       </c>
       <c r="F5">
-        <v>1298802944</v>
+        <v>1989004800</v>
       </c>
       <c r="G5">
-        <v>4263078912</v>
+        <v>3954214912</v>
       </c>
       <c r="H5">
-        <v>5561881856</v>
+        <v>3373531136</v>
       </c>
       <c r="I5">
-        <v>9111191552</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>16</v>
+        <v>1818068326.4000001</v>
+      </c>
+      <c r="J5">
+        <v>1798175027.2</v>
+      </c>
+      <c r="K5">
+        <v>4986184192</v>
+      </c>
+      <c r="L5">
+        <v>1279812352</v>
+      </c>
+      <c r="M5">
+        <v>1053608192</v>
+      </c>
+      <c r="N5">
+        <v>10575848652.799999</v>
+      </c>
+      <c r="O5">
+        <v>7639985664</v>
+      </c>
+      <c r="P5">
+        <v>4247731456</v>
+      </c>
+      <c r="Q5">
+        <v>5069071872</v>
+      </c>
+      <c r="R5">
+        <v>12374023680</v>
+      </c>
+      <c r="S5">
+        <v>12626169856</v>
+      </c>
+      <c r="T5">
+        <v>5527543808</v>
+      </c>
+      <c r="U5">
+        <v>6122680064</v>
+      </c>
+      <c r="V5">
+        <v>14363028480</v>
+      </c>
+      <c r="W5">
+        <v>16580384768</v>
+      </c>
+      <c r="X5">
+        <v>8901074944</v>
+      </c>
+      <c r="Y5">
+        <v>7940748390.3999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>12229745664</v>
+      </c>
+      <c r="C6">
+        <v>14734629888</v>
       </c>
       <c r="D6">
-        <v>6035295488</v>
+        <v>5734436352</v>
       </c>
       <c r="E6">
-        <v>1691007846.4000001</v>
+        <v>6074340352</v>
       </c>
       <c r="F6">
-        <v>1047843993.6</v>
+        <v>2052150272</v>
       </c>
       <c r="G6">
-        <v>4987451494.3999996</v>
+        <v>2889996902.4000001</v>
       </c>
       <c r="H6">
-        <v>6035295488</v>
+        <v>3345331916.8000002</v>
       </c>
       <c r="I6">
-        <v>772630334</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+        <v>1667566080</v>
+      </c>
+      <c r="J6">
+        <v>4508890624</v>
+      </c>
+      <c r="K6">
+        <v>5396388864</v>
+      </c>
+      <c r="L6">
+        <v>1417990144</v>
+      </c>
+      <c r="M6">
+        <v>1037419315.2</v>
+      </c>
+      <c r="N6">
+        <v>7720855040</v>
+      </c>
+      <c r="O6">
+        <v>9338241024</v>
+      </c>
+      <c r="P6">
+        <v>4316446208</v>
+      </c>
+      <c r="Q6">
+        <v>5036921036.8000002</v>
+      </c>
+      <c r="R6">
+        <v>12229745664</v>
+      </c>
+      <c r="S6">
+        <v>14734629888</v>
+      </c>
+      <c r="T6">
+        <v>5734436352</v>
+      </c>
+      <c r="U6">
+        <v>6074340352</v>
+      </c>
+      <c r="V6">
+        <v>14281895936</v>
+      </c>
+      <c r="W6">
+        <v>17624626790.400002</v>
+      </c>
+      <c r="X6">
+        <v>9079768268.7999992</v>
+      </c>
+      <c r="Y6">
+        <v>7741906432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>12418041856</v>
+      </c>
+      <c r="C7">
+        <v>11582755328</v>
+      </c>
+      <c r="D7">
+        <v>6036985856</v>
+      </c>
+      <c r="E7">
+        <v>6140170240</v>
+      </c>
+      <c r="F7">
+        <v>1947080704</v>
+      </c>
+      <c r="G7">
+        <v>954430976</v>
+      </c>
+      <c r="H7">
+        <v>3324485632</v>
+      </c>
+      <c r="I7">
+        <v>1856379801.5999999</v>
+      </c>
+      <c r="J7">
+        <v>1717132288</v>
+      </c>
+      <c r="K7">
+        <v>832943616</v>
+      </c>
+      <c r="L7">
+        <v>1695774924.8</v>
+      </c>
+      <c r="M7">
+        <v>1055496704</v>
+      </c>
+      <c r="N7">
+        <v>10700909568</v>
+      </c>
+      <c r="O7">
+        <v>10749811712</v>
+      </c>
+      <c r="P7">
+        <v>4341210931.1999998</v>
+      </c>
+      <c r="Q7">
+        <v>5084673536</v>
+      </c>
+      <c r="R7">
+        <v>12418041856</v>
+      </c>
+      <c r="S7">
+        <v>11582755328</v>
+      </c>
+      <c r="T7">
+        <v>6036985856</v>
+      </c>
+      <c r="U7">
+        <v>6140170240</v>
+      </c>
+      <c r="V7">
+        <v>14365122560</v>
+      </c>
+      <c r="W7">
+        <v>12537186304</v>
+      </c>
+      <c r="X7">
+        <v>9361471488</v>
+      </c>
+      <c r="Y7">
+        <v>7996550041.6000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>12298442752</v>
+      </c>
+      <c r="C8">
+        <v>13057903616</v>
       </c>
       <c r="D8">
-        <v>8692855808</v>
+        <v>5382971392</v>
       </c>
       <c r="E8">
-        <v>2828185600</v>
+        <v>6149596160</v>
       </c>
       <c r="F8">
-        <v>2009430016</v>
+        <v>1941376000</v>
       </c>
       <c r="G8">
-        <v>6683425792</v>
+        <v>3597308928</v>
       </c>
       <c r="H8">
-        <v>8692855808</v>
+        <v>3507509248</v>
       </c>
       <c r="I8">
-        <v>11521041408</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>14</v>
+        <v>1860010803.2</v>
+      </c>
+      <c r="J8">
+        <v>1770470400</v>
+      </c>
+      <c r="K8">
+        <v>5264488448</v>
+      </c>
+      <c r="L8">
+        <v>1166428211.2</v>
+      </c>
+      <c r="M8">
+        <v>1080133632</v>
+      </c>
+      <c r="N8">
+        <v>10527972352</v>
+      </c>
+      <c r="O8">
+        <v>7793415168</v>
+      </c>
+      <c r="P8">
+        <v>4216543180.8000002</v>
+      </c>
+      <c r="Q8">
+        <v>5069462528</v>
+      </c>
+      <c r="R8">
+        <v>12298442752</v>
+      </c>
+      <c r="S8">
+        <v>13057903616</v>
+      </c>
+      <c r="T8">
+        <v>5382971392</v>
+      </c>
+      <c r="U8">
+        <v>6149596160</v>
+      </c>
+      <c r="V8">
+        <v>14239818752</v>
+      </c>
+      <c r="W8">
+        <v>16655212544</v>
+      </c>
+      <c r="X8">
+        <v>8890480640</v>
+      </c>
+      <c r="Y8">
+        <v>8009606963.1999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>12411387904</v>
+      </c>
+      <c r="C9">
+        <v>12178317312</v>
       </c>
       <c r="D9">
-        <v>14480795648</v>
+        <v>5664076800</v>
       </c>
       <c r="E9">
-        <v>3204681728</v>
+        <v>6067732480</v>
       </c>
       <c r="F9">
-        <v>6328422528</v>
+        <v>1923090432</v>
       </c>
       <c r="G9">
-        <v>8162373120</v>
+        <v>2790411264</v>
       </c>
       <c r="H9">
-        <v>14480795648</v>
+        <v>3478842163.1999998</v>
       </c>
       <c r="I9">
-        <v>17685477376</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>15</v>
+        <v>1672437760</v>
+      </c>
+      <c r="J9">
+        <v>1725591552</v>
+      </c>
+      <c r="K9">
+        <v>9674468864</v>
+      </c>
+      <c r="L9">
+        <v>1363543756.8</v>
+      </c>
+      <c r="M9">
+        <v>1003067392</v>
+      </c>
+      <c r="N9">
+        <v>10685796352</v>
+      </c>
+      <c r="O9">
+        <v>2503848448</v>
+      </c>
+      <c r="P9">
+        <v>4300533043.1999998</v>
+      </c>
+      <c r="Q9">
+        <v>5064665088</v>
+      </c>
+      <c r="R9">
+        <v>12411387904</v>
+      </c>
+      <c r="S9">
+        <v>12178317312</v>
+      </c>
+      <c r="T9">
+        <v>5664076800</v>
+      </c>
+      <c r="U9">
+        <v>6067732480</v>
+      </c>
+      <c r="V9">
+        <v>14334478336</v>
+      </c>
+      <c r="W9">
+        <v>14968728576</v>
+      </c>
+      <c r="X9">
+        <v>9142918963.2000008</v>
+      </c>
+      <c r="Y9">
+        <v>7740170240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>12398845952</v>
+      </c>
+      <c r="C10">
+        <v>10584549376</v>
       </c>
       <c r="D10">
-        <v>5923102720</v>
+        <v>6410221056</v>
       </c>
       <c r="E10">
-        <v>3335118848</v>
+        <v>6602087936</v>
       </c>
       <c r="F10">
-        <v>1591776526</v>
+        <v>1958672793.5999999</v>
       </c>
       <c r="G10">
-        <v>4331326464</v>
+        <v>1623934976</v>
       </c>
       <c r="H10">
-        <v>5923102720</v>
+        <v>3097109811.1999998</v>
       </c>
       <c r="I10">
-        <v>9258221568</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>16</v>
+        <v>1711957504</v>
+      </c>
+      <c r="J10">
+        <v>1765707366.4000001</v>
+      </c>
+      <c r="K10">
+        <v>2638219776</v>
+      </c>
+      <c r="L10">
+        <v>1615952998.4000001</v>
+      </c>
+      <c r="M10">
+        <v>1107687424</v>
+      </c>
+      <c r="N10">
+        <v>10633138585.599899</v>
+      </c>
+      <c r="O10">
+        <v>7946329600</v>
+      </c>
+      <c r="P10">
+        <v>4794268057.6000004</v>
+      </c>
+      <c r="Q10">
+        <v>5494400512</v>
+      </c>
+      <c r="R10">
+        <v>12398845952</v>
+      </c>
+      <c r="S10">
+        <v>10584549376</v>
+      </c>
+      <c r="T10">
+        <v>6410221056</v>
+      </c>
+      <c r="U10">
+        <v>6602087936</v>
+      </c>
+      <c r="V10">
+        <v>14357518745.6</v>
+      </c>
+      <c r="W10">
+        <v>12208484352</v>
+      </c>
+      <c r="X10">
+        <v>9507330867.2000008</v>
+      </c>
+      <c r="Y10">
+        <v>8314045440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>11799913472</v>
+      </c>
+      <c r="C11">
+        <v>39678611456</v>
       </c>
       <c r="D11">
-        <v>6038848512</v>
+        <v>5603912704</v>
       </c>
       <c r="E11">
-        <v>1656857190.4000001</v>
+        <v>6090464256</v>
       </c>
       <c r="F11">
-        <v>1012921856</v>
+        <v>2230175744</v>
       </c>
       <c r="G11">
-        <v>5025926656</v>
+        <v>14794378444.799999</v>
       </c>
       <c r="H11">
-        <v>6038848512</v>
+        <v>3552331776</v>
       </c>
       <c r="I11">
-        <v>7695705702.3999996</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
+        <v>1636614656</v>
+      </c>
+      <c r="J11">
+        <v>4635690086.3999996</v>
+      </c>
+      <c r="K11">
+        <v>35226010112</v>
+      </c>
+      <c r="L11">
+        <v>1337819136</v>
+      </c>
+      <c r="M11">
+        <v>1049217024</v>
+      </c>
+      <c r="N11">
+        <v>7164223385.6000004</v>
+      </c>
+      <c r="O11">
+        <v>4452601344</v>
+      </c>
+      <c r="P11">
+        <v>4266093568</v>
+      </c>
+      <c r="Q11">
+        <v>5041247232</v>
+      </c>
+      <c r="R11">
+        <v>11799913472</v>
+      </c>
+      <c r="S11">
+        <v>39678611456</v>
+      </c>
+      <c r="T11">
+        <v>5603912704</v>
+      </c>
+      <c r="U11">
+        <v>6090464256</v>
+      </c>
+      <c r="V11">
+        <v>14030089216</v>
+      </c>
+      <c r="W11">
+        <v>54472989900.800003</v>
+      </c>
+      <c r="X11">
+        <v>9156244480</v>
+      </c>
+      <c r="Y11">
+        <v>7727078912</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>12379942912</v>
+      </c>
+      <c r="C12">
+        <v>9290638336</v>
+      </c>
+      <c r="D12">
+        <v>5798306304</v>
+      </c>
+      <c r="E12">
+        <v>6596495872</v>
+      </c>
+      <c r="F12">
+        <v>1958896435.2</v>
+      </c>
+      <c r="G12">
+        <v>4489060352</v>
+      </c>
+      <c r="H12">
+        <v>3499166208</v>
+      </c>
+      <c r="I12">
+        <v>1666368512</v>
+      </c>
+      <c r="J12">
+        <v>1710077952</v>
+      </c>
+      <c r="K12">
+        <v>6973896192</v>
+      </c>
+      <c r="L12">
+        <v>1468101632</v>
+      </c>
+      <c r="M12">
+        <v>1116552192</v>
+      </c>
+      <c r="N12">
+        <v>10669864960</v>
+      </c>
+      <c r="O12">
+        <v>2316742144</v>
+      </c>
+      <c r="P12">
+        <v>4330204672</v>
+      </c>
+      <c r="Q12">
+        <v>5479943680</v>
+      </c>
+      <c r="R12">
+        <v>12379942912</v>
+      </c>
+      <c r="S12">
+        <v>9290638336</v>
+      </c>
+      <c r="T12">
+        <v>5798306304</v>
+      </c>
+      <c r="U12">
+        <v>6596495872</v>
+      </c>
+      <c r="V12">
+        <v>14338839347.200001</v>
+      </c>
+      <c r="W12">
+        <v>13779698688</v>
+      </c>
+      <c r="X12">
+        <v>9297472512</v>
+      </c>
+      <c r="Y12">
+        <v>8262864384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>18193276928</v>
+      </c>
+      <c r="C13">
+        <v>12541907968</v>
       </c>
       <c r="D13">
-        <v>12349798400</v>
+        <v>5764779008</v>
       </c>
       <c r="E13">
-        <v>1978885120</v>
+        <v>9792070656</v>
       </c>
       <c r="F13">
-        <v>1746161049.5999999</v>
+        <v>4136850227.1999998</v>
       </c>
       <c r="G13">
-        <v>10603637350.4</v>
+        <v>6549722112</v>
       </c>
       <c r="H13">
-        <v>12349798400</v>
+        <v>3464335360</v>
       </c>
       <c r="I13">
-        <v>14328683520</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14">
-        <v>2680420608</v>
-      </c>
-      <c r="E14">
-        <v>8086517504</v>
-      </c>
-      <c r="F14">
-        <v>546768768</v>
-      </c>
-      <c r="G14">
-        <v>2133651840</v>
-      </c>
-      <c r="H14">
-        <v>2680420608</v>
-      </c>
-      <c r="I14">
-        <v>10766938112</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>5790441472</v>
-      </c>
-      <c r="E15">
-        <v>3468123340.8000002</v>
-      </c>
-      <c r="F15">
-        <v>1514427904</v>
-      </c>
-      <c r="G15">
-        <v>4276013568</v>
-      </c>
-      <c r="H15">
-        <v>5790441472</v>
-      </c>
-      <c r="I15">
-        <v>9258564812.7999992</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16">
-        <v>6081265664</v>
-      </c>
-      <c r="E16">
-        <v>1648764313.5999999</v>
-      </c>
-      <c r="F16">
-        <v>1057875456</v>
-      </c>
-      <c r="G16">
-        <v>5023390208</v>
-      </c>
-      <c r="H16">
-        <v>6081265664</v>
-      </c>
-      <c r="I16">
-        <v>7730029977.6000004</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <v>12374023680</v>
-      </c>
-      <c r="E18">
-        <v>1989004800</v>
-      </c>
-      <c r="F18">
-        <v>1798175027.2</v>
-      </c>
-      <c r="G18">
-        <v>10575848652.799999</v>
-      </c>
-      <c r="H18">
-        <v>12374023680</v>
-      </c>
-      <c r="I18">
-        <v>14363028480</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19">
-        <v>12626169856</v>
-      </c>
-      <c r="E19">
-        <v>3954214912</v>
-      </c>
-      <c r="F19">
-        <v>4986184192</v>
-      </c>
-      <c r="G19">
-        <v>7639985664</v>
-      </c>
-      <c r="H19">
-        <v>12626169856</v>
-      </c>
-      <c r="I19">
-        <v>16580384768</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20">
-        <v>5527543808</v>
-      </c>
-      <c r="E20">
-        <v>3373531136</v>
-      </c>
-      <c r="F20">
-        <v>1279812352</v>
-      </c>
-      <c r="G20">
-        <v>4247731456</v>
-      </c>
-      <c r="H20">
-        <v>5527543808</v>
-      </c>
-      <c r="I20">
-        <v>8901074944</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21">
-        <v>6122680064</v>
-      </c>
-      <c r="E21">
-        <v>1818068326.4000001</v>
-      </c>
-      <c r="F21">
-        <v>1053608192</v>
-      </c>
-      <c r="G21">
-        <v>5069071872</v>
-      </c>
-      <c r="H21">
-        <v>6122680064</v>
-      </c>
-      <c r="I21">
-        <v>7940748390.3999996</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23">
-        <v>12229745664</v>
-      </c>
-      <c r="E23">
-        <v>2052150272</v>
-      </c>
-      <c r="F23">
-        <v>4508890624</v>
-      </c>
-      <c r="G23">
-        <v>7720855040</v>
-      </c>
-      <c r="H23">
-        <v>12229745664</v>
-      </c>
-      <c r="I23">
-        <v>14281895936</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24">
-        <v>14734629888</v>
-      </c>
-      <c r="E24">
-        <v>2889996902.4000001</v>
-      </c>
-      <c r="F24">
-        <v>5396388864</v>
-      </c>
-      <c r="G24">
-        <v>9338241024</v>
-      </c>
-      <c r="H24">
-        <v>14734629888</v>
-      </c>
-      <c r="I24">
-        <v>17624626790.400002</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25">
-        <v>5734436352</v>
-      </c>
-      <c r="E25">
-        <v>3345331916.8000002</v>
-      </c>
-      <c r="F25">
-        <v>1417990144</v>
-      </c>
-      <c r="G25">
-        <v>4316446208</v>
-      </c>
-      <c r="H25">
-        <v>5734436352</v>
-      </c>
-      <c r="I25">
-        <v>9079768268.7999992</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26">
-        <v>6074340352</v>
-      </c>
-      <c r="E26">
-        <v>1667566080</v>
-      </c>
-      <c r="F26">
-        <v>1037419315.2</v>
-      </c>
-      <c r="G26">
-        <v>5036921036.8000002</v>
-      </c>
-      <c r="H26">
-        <v>6074340352</v>
-      </c>
-      <c r="I26">
-        <v>7741906432</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28">
-        <v>12418041856</v>
-      </c>
-      <c r="E28">
-        <v>1947080704</v>
-      </c>
-      <c r="F28">
-        <v>1717132288</v>
-      </c>
-      <c r="G28">
-        <v>10700909568</v>
-      </c>
-      <c r="H28">
-        <v>12418041856</v>
-      </c>
-      <c r="I28">
-        <v>14365122560</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29">
-        <v>11582755328</v>
-      </c>
-      <c r="E29">
-        <v>954430976</v>
-      </c>
-      <c r="F29">
-        <v>832943616</v>
-      </c>
-      <c r="G29">
-        <v>10749811712</v>
-      </c>
-      <c r="H29">
-        <v>11582755328</v>
-      </c>
-      <c r="I29">
-        <v>12537186304</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30">
-        <v>6036985856</v>
-      </c>
-      <c r="E30">
-        <v>3324485632</v>
-      </c>
-      <c r="F30">
-        <v>1695774924.8</v>
-      </c>
-      <c r="G30">
-        <v>4341210931.1999998</v>
-      </c>
-      <c r="H30">
-        <v>6036985856</v>
-      </c>
-      <c r="I30">
-        <v>9361471488</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31">
-        <v>6140170240</v>
-      </c>
-      <c r="E31">
-        <v>1856379801.5999999</v>
-      </c>
-      <c r="F31">
-        <v>1055496704</v>
-      </c>
-      <c r="G31">
-        <v>5084673536</v>
-      </c>
-      <c r="H31">
-        <v>6140170240</v>
-      </c>
-      <c r="I31">
-        <v>7996550041.6000004</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33">
-        <v>12298442752</v>
-      </c>
-      <c r="E33">
-        <v>1941376000</v>
-      </c>
-      <c r="F33">
-        <v>1770470400</v>
-      </c>
-      <c r="G33">
-        <v>10527972352</v>
-      </c>
-      <c r="H33">
-        <v>12298442752</v>
-      </c>
-      <c r="I33">
-        <v>14239818752</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34">
-        <v>13057903616</v>
-      </c>
-      <c r="E34">
-        <v>3597308928</v>
-      </c>
-      <c r="F34">
-        <v>5264488448</v>
-      </c>
-      <c r="G34">
-        <v>7793415168</v>
-      </c>
-      <c r="H34">
-        <v>13057903616</v>
-      </c>
-      <c r="I34">
-        <v>16655212544</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35">
-        <v>5382971392</v>
-      </c>
-      <c r="E35">
-        <v>3507509248</v>
-      </c>
-      <c r="F35">
-        <v>1166428211.2</v>
-      </c>
-      <c r="G35">
-        <v>4216543180.8000002</v>
-      </c>
-      <c r="H35">
-        <v>5382971392</v>
-      </c>
-      <c r="I35">
-        <v>8890480640</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36">
-        <v>6149596160</v>
-      </c>
-      <c r="E36">
-        <v>1860010803.2</v>
-      </c>
-      <c r="F36">
-        <v>1080133632</v>
-      </c>
-      <c r="G36">
-        <v>5069462528</v>
-      </c>
-      <c r="H36">
-        <v>6149596160</v>
-      </c>
-      <c r="I36">
-        <v>8009606963.1999998</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38">
-        <v>12411387904</v>
-      </c>
-      <c r="E38">
-        <v>1923090432</v>
-      </c>
-      <c r="F38">
-        <v>1725591552</v>
-      </c>
-      <c r="G38">
-        <v>10685796352</v>
-      </c>
-      <c r="H38">
-        <v>12411387904</v>
-      </c>
-      <c r="I38">
-        <v>14334478336</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39">
-        <v>12178317312</v>
-      </c>
-      <c r="E39">
-        <v>2790411264</v>
-      </c>
-      <c r="F39">
-        <v>9674468864</v>
-      </c>
-      <c r="G39">
-        <v>2503848448</v>
-      </c>
-      <c r="H39">
-        <v>12178317312</v>
-      </c>
-      <c r="I39">
-        <v>14968728576</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40">
-        <v>5664076800</v>
-      </c>
-      <c r="E40">
-        <v>3478842163.1999998</v>
-      </c>
-      <c r="F40">
-        <v>1363543756.8</v>
-      </c>
-      <c r="G40">
-        <v>4300533043.1999998</v>
-      </c>
-      <c r="H40">
-        <v>5664076800</v>
-      </c>
-      <c r="I40">
-        <v>9142918963.2000008</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41">
-        <v>6067732480</v>
-      </c>
-      <c r="E41">
-        <v>1672437760</v>
-      </c>
-      <c r="F41">
-        <v>1003067392</v>
-      </c>
-      <c r="G41">
-        <v>5064665088</v>
-      </c>
-      <c r="H41">
-        <v>6067732480</v>
-      </c>
-      <c r="I41">
-        <v>7740170240</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43">
-        <v>12398845952</v>
-      </c>
-      <c r="E43">
-        <v>1958672793.5999999</v>
-      </c>
-      <c r="F43">
-        <v>1765707366.4000001</v>
-      </c>
-      <c r="G43">
-        <v>10633138585.599899</v>
-      </c>
-      <c r="H43">
-        <v>12398845952</v>
-      </c>
-      <c r="I43">
-        <v>14357518745.6</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44">
-        <v>10584549376</v>
-      </c>
-      <c r="E44">
-        <v>1623934976</v>
-      </c>
-      <c r="F44">
-        <v>2638219776</v>
-      </c>
-      <c r="G44">
-        <v>7946329600</v>
-      </c>
-      <c r="H44">
-        <v>10584549376</v>
-      </c>
-      <c r="I44">
-        <v>12208484352</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45">
-        <v>6410221056</v>
-      </c>
-      <c r="E45">
-        <v>3097109811.1999998</v>
-      </c>
-      <c r="F45">
-        <v>1615952998.4000001</v>
-      </c>
-      <c r="G45">
-        <v>4794268057.6000004</v>
-      </c>
-      <c r="H45">
-        <v>6410221056</v>
-      </c>
-      <c r="I45">
-        <v>9507330867.2000008</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46">
-        <v>6602087936</v>
-      </c>
-      <c r="E46">
-        <v>1711957504</v>
-      </c>
-      <c r="F46">
-        <v>1107687424</v>
-      </c>
-      <c r="G46">
-        <v>5494400512</v>
-      </c>
-      <c r="H46">
-        <v>6602087936</v>
-      </c>
-      <c r="I46">
-        <v>8314045440</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D48">
-        <v>11799913472</v>
-      </c>
-      <c r="E48">
-        <v>2230175744</v>
-      </c>
-      <c r="F48">
-        <v>4635690086.3999996</v>
-      </c>
-      <c r="G48">
-        <v>7164223385.6000004</v>
-      </c>
-      <c r="H48">
-        <v>11799913472</v>
-      </c>
-      <c r="I48">
-        <v>14030089216</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49">
-        <v>39678611456</v>
-      </c>
-      <c r="E49">
-        <v>14794378444.799999</v>
-      </c>
-      <c r="F49">
-        <v>35226010112</v>
-      </c>
-      <c r="G49">
-        <v>4452601344</v>
-      </c>
-      <c r="H49">
-        <v>39678611456</v>
-      </c>
-      <c r="I49">
-        <v>54472989900.800003</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50">
-        <v>5603912704</v>
-      </c>
-      <c r="E50">
-        <v>3552331776</v>
-      </c>
-      <c r="F50">
-        <v>1337819136</v>
-      </c>
-      <c r="G50">
-        <v>4266093568</v>
-      </c>
-      <c r="H50">
-        <v>5603912704</v>
-      </c>
-      <c r="I50">
-        <v>9156244480</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51">
-        <v>6090464256</v>
-      </c>
-      <c r="E51">
-        <v>1636614656</v>
-      </c>
-      <c r="F51">
-        <v>1049217024</v>
-      </c>
-      <c r="G51">
-        <v>5041247232</v>
-      </c>
-      <c r="H51">
-        <v>6090464256</v>
-      </c>
-      <c r="I51">
-        <v>7727078912</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53">
-        <v>12379942912</v>
-      </c>
-      <c r="E53">
-        <v>1958896435.2</v>
-      </c>
-      <c r="F53">
-        <v>1710077952</v>
-      </c>
-      <c r="G53">
-        <v>10669864960</v>
-      </c>
-      <c r="H53">
-        <v>12379942912</v>
-      </c>
-      <c r="I53">
-        <v>14338839347.200001</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54">
-        <v>9290638336</v>
-      </c>
-      <c r="E54">
-        <v>4489060352</v>
-      </c>
-      <c r="F54">
-        <v>6973896192</v>
-      </c>
-      <c r="G54">
-        <v>2316742144</v>
-      </c>
-      <c r="H54">
-        <v>9290638336</v>
-      </c>
-      <c r="I54">
-        <v>13779698688</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55">
-        <v>5798306304</v>
-      </c>
-      <c r="E55">
-        <v>3499166208</v>
-      </c>
-      <c r="F55">
-        <v>1468101632</v>
-      </c>
-      <c r="G55">
-        <v>4330204672</v>
-      </c>
-      <c r="H55">
-        <v>5798306304</v>
-      </c>
-      <c r="I55">
-        <v>9297472512</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C56" t="s">
-        <v>16</v>
-      </c>
-      <c r="D56">
-        <v>6596495872</v>
-      </c>
-      <c r="E56">
-        <v>1666368512</v>
-      </c>
-      <c r="F56">
-        <v>1116552192</v>
-      </c>
-      <c r="G56">
-        <v>5479943680</v>
-      </c>
-      <c r="H56">
-        <v>6596495872</v>
-      </c>
-      <c r="I56">
-        <v>8262864384</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58">
+        <v>2264098816</v>
+      </c>
+      <c r="J13">
+        <v>3700474880</v>
+      </c>
+      <c r="K13">
+        <v>11274372992</v>
+      </c>
+      <c r="L13">
+        <v>1432443904</v>
+      </c>
+      <c r="M13">
+        <v>2211627520</v>
+      </c>
+      <c r="N13">
+        <v>14492802048</v>
+      </c>
+      <c r="O13">
+        <v>1267534976</v>
+      </c>
+      <c r="P13">
+        <v>4332335104</v>
+      </c>
+      <c r="Q13">
+        <v>7580443136</v>
+      </c>
+      <c r="R13">
         <v>18193276928</v>
       </c>
-      <c r="E58">
-        <v>4136850227.1999998</v>
-      </c>
-      <c r="F58">
-        <v>3700474880</v>
-      </c>
-      <c r="G58">
-        <v>14492802048</v>
-      </c>
-      <c r="H58">
-        <v>18193276928</v>
-      </c>
-      <c r="I58">
+      <c r="S13">
+        <v>12541907968</v>
+      </c>
+      <c r="T13">
+        <v>5764779008</v>
+      </c>
+      <c r="U13">
+        <v>9792070656</v>
+      </c>
+      <c r="V13">
         <v>22330127155.200001</v>
       </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C59" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59">
-        <v>12541907968</v>
-      </c>
-      <c r="E59">
-        <v>6549722112</v>
-      </c>
-      <c r="F59">
-        <v>11274372992</v>
-      </c>
-      <c r="G59">
-        <v>1267534976</v>
-      </c>
-      <c r="H59">
-        <v>12541907968</v>
-      </c>
-      <c r="I59">
+      <c r="W13">
         <v>19091630080</v>
       </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>5764779008</v>
-      </c>
-      <c r="E60">
-        <v>3464335360</v>
-      </c>
-      <c r="F60">
-        <v>1432443904</v>
-      </c>
-      <c r="G60">
-        <v>4332335104</v>
-      </c>
-      <c r="H60">
-        <v>5764779008</v>
-      </c>
-      <c r="I60">
+      <c r="X13">
         <v>9229114368</v>
       </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C61" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61">
-        <v>9792070656</v>
-      </c>
-      <c r="E61">
-        <v>2264098816</v>
-      </c>
-      <c r="F61">
-        <v>2211627520</v>
-      </c>
-      <c r="G61">
-        <v>7580443136</v>
-      </c>
-      <c r="H61">
-        <v>9792070656</v>
-      </c>
-      <c r="I61">
+      <c r="Y13">
         <v>12056169472</v>
       </c>
     </row>
@@ -1630,22 +1551,22 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
@@ -2798,7 +2719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -2820,22 +2741,22 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">

</xml_diff>